<commit_message>
Entered all points, now just finishing w ludwig
Signed-off-by: Maximilian von Tschirschnitz <tschirschnitz@sec.in.tum.de>
</commit_message>
<xml_diff>
--- a/bewertung_ws22.xlsx
+++ b/bewertung_ws22.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Contents</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Pfanz</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Zinn</t>
   </si>
   <si>
@@ -88,51 +85,21 @@
     <t>0</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Otting</t>
   </si>
   <si>
-    <t>25</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Rammouz</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Haberl</t>
   </si>
   <si>
-    <t>21-22</t>
-  </si>
-  <si>
     <t>Mayer</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Schweinhuber</t>
   </si>
   <si>
@@ -142,10 +109,28 @@
     <t>Stillmark</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Buhl</t>
+  </si>
+  <si>
+    <t>Blaschko</t>
+  </si>
+  <si>
+    <t>Ebert</t>
+  </si>
+  <si>
+    <t>Schaffland</t>
+  </si>
+  <si>
+    <t>Vasudevan</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>5-6</t>
   </si>
 </sst>
 </file>
@@ -157,7 +142,7 @@
     <numFmt numFmtId="165" formatCode="0.0;[Red]0.0"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +261,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Dejavu"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Dejavu"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,8 +354,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -439,6 +451,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -463,7 +488,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -481,7 +506,6 @@
     <xf numFmtId="164" fontId="14" fillId="9" borderId="6" xfId="18" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="18" applyBorder="1"/>
     <xf numFmtId="165" fontId="16" fillId="10" borderId="0" xfId="20" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="20"/>
     <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="20" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="16" fillId="10" borderId="6" xfId="20" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="16" fillId="10" borderId="0" xfId="20" applyNumberFormat="1" applyBorder="1"/>
@@ -496,13 +520,79 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="6" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="10" borderId="0" xfId="20" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="10" borderId="0" xfId="20" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="6" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="6" xfId="18" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="7" xfId="18" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="18" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Accent" xfId="2"/>
@@ -826,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -838,9 +928,9 @@
     <col min="4" max="5" width="8.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="2.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.875" style="1" customWidth="1"/>
     <col min="13" max="13" width="2.5" style="1" customWidth="1"/>
@@ -950,22 +1040,22 @@
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="25">
         <v>25</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>9</v>
       </c>
-      <c r="D3" s="26">
-        <v>5</v>
-      </c>
-      <c r="E3" s="26">
-        <v>5</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="26"/>
+      <c r="D3" s="25">
+        <v>5</v>
+      </c>
+      <c r="E3" s="25">
+        <v>5</v>
+      </c>
+      <c r="F3" s="25">
+        <v>2</v>
+      </c>
+      <c r="G3" s="25"/>
       <c r="H3" s="14"/>
       <c r="I3" s="5">
         <f t="shared" ref="I3:I29" si="0">IF(ISNUMBER(G3), $G$2 +  0.8 * SUM($B$2:$F$2),SUM($B$2:$F$2))</f>
@@ -973,57 +1063,61 @@
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J11" si="1">IF(ISNUMBER(G3), G3 + SUM(B3:F3) * 0.8,SUM(B3:F3))</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K3" s="5">
-        <f t="shared" ref="K3:K11" si="2">MIN(1+(ROUNDDOWN(((I3-J3))/(I3/20),0)*(1/3)),5)</f>
-        <v>1.6666666666666665</v>
+        <f>MIN(1+(ROUNDDOWN(((I3-J3))/(I3/20),0)*(1/3)),5)</f>
+        <v>1.3333333333333333</v>
       </c>
       <c r="L3" s="5">
-        <f t="shared" ref="L3:L11" si="3">IF(K3&gt;1, I3 - ((K3-1) * 3 * (I3 / 20)) - J3, "X")</f>
-        <v>1</v>
+        <f t="shared" ref="L3:L11" si="2">IF(K3&gt;1, I3 - ((K3-1) * 3 * (I3 / 20)) - J3, "X")</f>
+        <v>1.5</v>
       </c>
       <c r="M3" s="14"/>
-      <c r="N3"/>
-      <c r="O3" s="21"/>
+      <c r="N3" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="36">
+        <v>40</v>
+      </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="5">
-        <f t="shared" ref="Q3:Q11" si="4">I3+N$2+O$2</f>
+        <f t="shared" ref="Q3:Q11" si="3">I3+N$2+O$2</f>
         <v>100</v>
       </c>
       <c r="R3" s="5">
         <f>IF(ISNUMBER(#REF!), J3*0.8+#REF! +N3+O3, J3+N3+O3)</f>
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="S3" s="5">
-        <f t="shared" ref="S3:S11" si="5">MIN(1+(ROUNDDOWN(((Q3-R3))/(Q3/20),0)*(1/3)),5)</f>
-        <v>4.6666666666666661</v>
-      </c>
-      <c r="T3" s="5">
-        <f t="shared" ref="T3:T11" si="6">IF(S3&gt;1, Q3 - ((S3-1) * 3 * (Q3 / 20)) - R3, "X")</f>
-        <v>1.0000000000000071</v>
+        <f t="shared" ref="S3:S11" si="4">MIN(1+(ROUNDDOWN(((Q3-R3))/(Q3/20),0)*(1/3)),5)</f>
+        <v>1</v>
+      </c>
+      <c r="T3" s="5" t="str">
+        <f t="shared" ref="T3:T11" si="5">IF(S3&gt;1, Q3 - ((S3-1) * 3 * (Q3 / 20)) - R3, "X")</f>
+        <v>X</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="25">
+        <v>10</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="26">
-        <v>10</v>
-      </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="E4" s="25">
+        <v>3</v>
+      </c>
+      <c r="F4" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="26">
-        <v>3</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="14"/>
       <c r="I4" s="5">
         <f t="shared" si="0"/>
@@ -1034,54 +1128,58 @@
         <v>13</v>
       </c>
       <c r="K4" s="5">
+        <f t="shared" ref="K3:K11" si="6">MIN(1+(ROUNDDOWN(((I4-J4))/(I4/20),0)*(1/3)),5)</f>
+        <v>5</v>
+      </c>
+      <c r="L4" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L4" s="5">
-        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="M4" s="14"/>
-      <c r="N4"/>
-      <c r="O4"/>
+      <c r="N4" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4">
+        <v>32</v>
+      </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="R4" s="5">
         <f>IF(ISNUMBER(#REF!), J4*0.8+#REF! +N4+O4, J4+N4+O4)</f>
-        <v>13</v>
+        <v>45097</v>
       </c>
       <c r="S4" s="5">
+        <f t="shared" si="4"/>
+        <v>-2998.6666666666665</v>
+      </c>
+      <c r="T4" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="T4" s="5">
-        <f t="shared" si="6"/>
-        <v>27</v>
+        <v>X</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15">
-      <c r="A5" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="27">
+      <c r="A5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="26">
         <v>25</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>10</v>
       </c>
-      <c r="D5" s="27">
-        <v>5</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="27">
-        <v>5</v>
-      </c>
-      <c r="G5" s="26"/>
+      <c r="D5" s="26">
+        <v>5</v>
+      </c>
+      <c r="E5" s="54">
+        <v>5</v>
+      </c>
+      <c r="F5" s="54">
+        <v>5</v>
+      </c>
+      <c r="G5" s="25"/>
       <c r="H5" s="14"/>
       <c r="I5" s="5">
         <f t="shared" si="0"/>
@@ -1089,57 +1187,61 @@
       </c>
       <c r="J5" s="5">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K5" s="5">
         <f>MIN(1+(ROUNDDOWN(((I5-J5))/(I5/20),0)*(1/3)),5)</f>
-        <v>1.6666666666666665</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L5" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
       </c>
       <c r="M5" s="14"/>
-      <c r="N5"/>
-      <c r="O5"/>
+      <c r="N5" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="55">
+        <v>40</v>
+      </c>
       <c r="P5" s="14"/>
       <c r="Q5" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="R5" s="5">
         <f>IF(ISNUMBER(#REF!), J5*0.8+#REF! +N5+O5, J5+N5+O5)</f>
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="S5" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T5" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>4.6666666666666661</v>
-      </c>
-      <c r="T5" s="5">
-        <f t="shared" si="6"/>
-        <v>7.1054273576010019E-15</v>
+        <v>X</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="54">
         <v>25</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="27"/>
+      <c r="C6" s="54">
+        <v>9</v>
+      </c>
+      <c r="D6" s="54">
+        <v>5</v>
+      </c>
+      <c r="E6" s="54">
+        <v>4</v>
+      </c>
+      <c r="F6" s="54">
+        <v>3</v>
+      </c>
+      <c r="G6" s="26"/>
       <c r="H6" s="14"/>
       <c r="I6" s="5">
         <f t="shared" si="0"/>
@@ -1147,173 +1249,185 @@
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K6" s="5">
+        <f t="shared" si="6"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L6" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L6" s="5">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <v>1.5</v>
       </c>
       <c r="M6" s="14"/>
-      <c r="N6"/>
-      <c r="O6"/>
+      <c r="N6" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6">
+        <v>40</v>
+      </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="R6" s="5">
         <f>IF(ISNUMBER(#REF!), J6*0.8+#REF! +N6+O6, J6+N6+O6)</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="S6" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T6" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="T6" s="5">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <v>X</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="5">
+      <c r="A7" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="56">
+        <v>18</v>
+      </c>
+      <c r="C7" s="56">
+        <v>8</v>
+      </c>
+      <c r="D7" s="56">
+        <v>5</v>
+      </c>
+      <c r="E7" s="56">
+        <v>3</v>
+      </c>
+      <c r="F7" s="56">
+        <v>2</v>
+      </c>
+      <c r="G7" s="46"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
+        <v>36</v>
+      </c>
+      <c r="K7" s="48">
+        <f t="shared" si="6"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="L7" s="48">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L7" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="M7" s="47"/>
+      <c r="N7" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="49">
+        <v>28</v>
+      </c>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="48">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="M7" s="14"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="5">
+        <v>100</v>
+      </c>
+      <c r="R7" s="48">
+        <f>IF(ISNUMBER(#REF!), J7*0.8+#REF! +N7+O7, J7+N7+O7)</f>
+        <v>64</v>
+      </c>
+      <c r="S7" s="48">
         <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="R7" s="5">
-        <f>IF(ISNUMBER(#REF!), J7*0.8+#REF! +N7+O7, J7+N7+O7)</f>
-        <v>0</v>
-      </c>
-      <c r="S7" s="5">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="T7" s="48">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="T7" s="5">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15">
-      <c r="A8" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31">
+      <c r="A8" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="58">
+        <v>22</v>
+      </c>
+      <c r="C8" s="58">
+        <v>9</v>
+      </c>
+      <c r="D8" s="58">
+        <v>5</v>
+      </c>
+      <c r="E8" s="58">
+        <v>4</v>
+      </c>
+      <c r="F8" s="58">
+        <v>5</v>
+      </c>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="29">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="29">
         <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="K8" s="29">
+        <f t="shared" si="6"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="L8" s="29">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K8" s="31">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L8" s="31">
+      <c r="M8" s="28"/>
+      <c r="N8" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="O8" s="30">
+        <v>40</v>
+      </c>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="29">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="M8" s="30"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="31">
+        <v>100</v>
+      </c>
+      <c r="R8" s="29">
+        <f>IF(ISNUMBER(#REF!), J8*0.8+#REF! +N8+O8, J8+N8+O8)</f>
+        <v>95</v>
+      </c>
+      <c r="S8" s="29">
         <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="R8" s="31">
-        <f>IF(ISNUMBER(#REF!), J8*0.8+#REF! +N8+O8, J8+N8+O8)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="T8" s="29">
+        <f t="shared" si="5"/>
         <v>0</v>
-      </c>
-      <c r="S8" s="31">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="T8" s="31">
-        <f t="shared" si="6"/>
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15">
       <c r="A9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="27"/>
+        <v>27</v>
+      </c>
+      <c r="B9" s="54">
+        <v>15</v>
+      </c>
+      <c r="C9" s="54">
+        <v>6</v>
+      </c>
+      <c r="D9" s="54">
+        <v>4</v>
+      </c>
+      <c r="E9" s="54">
+        <v>3</v>
+      </c>
+      <c r="F9" s="54">
+        <v>4</v>
+      </c>
+      <c r="G9" s="26"/>
       <c r="H9" s="14"/>
       <c r="I9" s="5">
         <f t="shared" si="0"/>
@@ -1321,57 +1435,61 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="K9" s="5">
+        <f t="shared" si="6"/>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L9" s="5">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <v>0.5</v>
       </c>
       <c r="M9" s="14"/>
-      <c r="N9"/>
-      <c r="O9"/>
+      <c r="N9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="60">
+        <v>28</v>
+      </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="R9" s="5">
         <f>IF(ISNUMBER(#REF!), J9*0.8+#REF! +N9+O9, J9+N9+O9)</f>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="S9" s="5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="T9" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="T9" s="5">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15">
-      <c r="A10" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="27" t="s">
+      <c r="A10" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="C10" s="54">
+        <v>8</v>
+      </c>
+      <c r="D10" s="54">
+        <v>3</v>
+      </c>
+      <c r="E10" s="54">
+        <v>4</v>
+      </c>
+      <c r="F10" s="54">
+        <v>2</v>
+      </c>
+      <c r="G10" s="26"/>
       <c r="H10" s="14"/>
       <c r="I10" s="5">
         <f t="shared" si="0"/>
@@ -1379,226 +1497,168 @@
       </c>
       <c r="J10" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K10" s="5">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="M10" s="14"/>
-      <c r="N10"/>
-      <c r="O10"/>
+      <c r="N10" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10">
+        <v>32</v>
+      </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="R10" s="5">
         <f>IF(ISNUMBER(#REF!), J10*0.8+#REF! +N10+O10, J10+N10+O10)</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="S10" s="5">
+        <f t="shared" si="4"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="T10" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="T10" s="5">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15">
-      <c r="A11" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="A11" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="54">
         <v>24</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="14"/>
+      <c r="C11" s="54">
+        <v>10</v>
+      </c>
+      <c r="D11" s="54">
+        <v>5</v>
+      </c>
+      <c r="E11" s="54">
+        <v>5</v>
+      </c>
+      <c r="F11" s="61">
+        <v>3</v>
+      </c>
+      <c r="G11" s="26"/>
+      <c r="H11" s="63"/>
       <c r="I11" s="5">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="K11" s="5">
+        <f t="shared" si="6"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="L11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="63"/>
+      <c r="N11" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11">
+        <v>35</v>
+      </c>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="5">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="M11" s="14"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="5">
-        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="R11" s="5">
         <f>IF(ISNUMBER(#REF!), J11*0.8+#REF! +N11+O11, J11+N11+O11)</f>
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="S11" s="5">
+        <f t="shared" si="4"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="T11" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="T11" s="5">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15">
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="5">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" ref="J12:J29" si="7">IF(ISNUMBER(G12), G12 + SUM(B12:F12) * 0.8,SUM(B12:F12))</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" ref="K12:K29" si="8">MIN(1+(ROUNDDOWN(((I12-J12))/(I12/20),0)*(1/3)),5)</f>
-        <v>5</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" ref="L12:L29" si="9">IF(K12&gt;1, I12 - ((K12-1) * 3 * (I12 / 20)) - J12, "X")</f>
-        <v>20</v>
-      </c>
-      <c r="M12" s="14"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="5">
-        <f t="shared" ref="Q12:Q29" si="10">I12+N$2+O$2</f>
-        <v>100</v>
-      </c>
-      <c r="R12" s="5">
-        <f>IF(ISNUMBER(#REF!), J12*0.8+#REF! +N12+O12, J12+N12+O12)</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="5">
-        <f t="shared" ref="S12:S29" si="11">MIN(1+(ROUNDDOWN(((Q12-R12))/(Q12/20),0)*(1/3)),5)</f>
-        <v>5</v>
-      </c>
-      <c r="T12" s="21">
-        <f t="shared" ref="T12:T29" si="12">IF(S12&gt;1, Q12 - ((S12-1) * 3 * (Q12 / 20)) - R12, "X")</f>
-        <v>40</v>
-      </c>
+      <c r="A12" s="64"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="62"/>
+      <c r="T12" s="69"/>
     </row>
     <row r="13" spans="1:20" ht="15">
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="5">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="M13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="5">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="R13" s="5">
-        <f>IF(ISNUMBER(#REF!), J13*0.8+#REF! +N13+O13, J13+N13+O13)</f>
-        <v>0</v>
-      </c>
-      <c r="S13" s="5">
-        <f t="shared" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="T13" s="5">
-        <f t="shared" si="12"/>
-        <v>40</v>
-      </c>
+      <c r="A13" s="64"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
     </row>
     <row r="14" spans="1:20" ht="15">
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="5">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J14" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="M14" s="15"/>
-      <c r="N14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="5">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="R14" s="5">
-        <f>IF(ISNUMBER(#REF!), J14*0.8+#REF! +N14+O14, J14+N14+O14)</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="5">
-        <f t="shared" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="T14" s="21">
-        <f t="shared" si="12"/>
-        <v>40</v>
-      </c>
+      <c r="A14" s="64"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="70"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="69"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="5"/>
@@ -1614,13 +1674,13 @@
         <v>50</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="J12:J29" si="7">IF(ISNUMBER(G15), G15 + SUM(B15:F15) * 0.8,SUM(B15:F15))</f>
         <v>0</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="N15" s="52"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
@@ -1648,7 +1708,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="N16" s="52"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
@@ -1676,7 +1736,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="N17" s="52"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -1685,13 +1745,25 @@
       <c r="T17" s="5"/>
     </row>
     <row r="18" spans="1:20" ht="15">
-      <c r="A18" s="4"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="26">
+        <v>24</v>
+      </c>
+      <c r="C18" s="54">
+        <v>8</v>
+      </c>
+      <c r="D18" s="54">
+        <v>5</v>
+      </c>
+      <c r="E18" s="54">
+        <v>5</v>
+      </c>
+      <c r="F18" s="54">
+        <v>5</v>
+      </c>
+      <c r="G18" s="26"/>
       <c r="H18" s="14"/>
       <c r="I18" s="5">
         <f>IF(ISNUMBER(G18), $G$2 +  0.8 * SUM($B$2:$F$2),SUM($B$2:$F$2))</f>
@@ -1699,22 +1771,22 @@
       </c>
       <c r="J18" s="5">
         <f>IF(ISNUMBER(G18), G18 + SUM(B18:F18) * 0.8,SUM(B18:F18))</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="K18" s="5">
         <f>MIN(1+(ROUNDDOWN(((I18-J18))/(I18/20),0)*(1/3)),5)</f>
-        <v>5</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="L18" s="5">
         <f>IF(K18&gt;1, I18 - ((K18-1) * 3 * (I18 / 20)) - J18, "X")</f>
-        <v>20</v>
+        <v>0.5</v>
       </c>
       <c r="M18" s="14"/>
-      <c r="N18">
-        <v>10</v>
+      <c r="N18" s="72">
+        <v>7</v>
       </c>
       <c r="O18">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="5">
@@ -1723,25 +1795,37 @@
       </c>
       <c r="R18" s="5">
         <f>J18+N18+O18</f>
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="S18" s="5">
         <f>MIN(1+(ROUNDDOWN(((Q18-R18))/(Q18/20),0)*(1/3)),5)</f>
-        <v>4.333333333333333</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="T18" s="5">
         <f>IF(S18&gt;1, Q18 - ((S18-1) * 3 * (Q18 / 20)) - R18, "X")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15">
+      <c r="A19" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="54">
+        <v>10</v>
+      </c>
+      <c r="C19" s="54">
+        <v>3</v>
+      </c>
+      <c r="D19" s="54">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="15">
-      <c r="A19" s="4"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
+      <c r="E19" s="54">
+        <v>2</v>
+      </c>
+      <c r="F19" s="54">
+        <v>3</v>
+      </c>
+      <c r="G19" s="26"/>
       <c r="H19" s="14"/>
       <c r="I19" s="5">
         <f>IF(ISNUMBER(G19), $G$2 +  0.8 * SUM($B$2:$F$2),SUM($B$2:$F$2))</f>
@@ -1749,7 +1833,7 @@
       </c>
       <c r="J19" s="5">
         <f>IF(ISNUMBER(G19), G19 + SUM(B19:F19) * 0.8,SUM(B19:F19))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K19" s="5">
         <f>MIN(1+(ROUNDDOWN(((I19-J19))/(I19/20),0)*(1/3)),5)</f>
@@ -1757,14 +1841,14 @@
       </c>
       <c r="L19" s="5">
         <f>IF(K19&gt;1, I19 - ((K19-1) * 3 * (I19 / 20)) - J19, "X")</f>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="M19" s="14"/>
-      <c r="N19">
-        <v>9</v>
-      </c>
-      <c r="O19">
-        <v>30</v>
+      <c r="N19" s="72">
+        <v>10</v>
+      </c>
+      <c r="O19" s="60">
+        <v>37</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="5">
@@ -1773,24 +1857,37 @@
       </c>
       <c r="R19" s="5">
         <f>IF(ISNUMBER(#REF!), J19*0.8+#REF! +N19+O19, J19+N19+O19)</f>
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="S19" s="5">
         <f>MIN(1+(ROUNDDOWN(((Q19-R19))/(Q19/20),0)*(1/3)),5)</f>
-        <v>5</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="T19" s="5">
         <f>IF(S19&gt;1, Q19 - ((S19-1) * 3 * (Q19 / 20)) - R19, "X")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="15">
-      <c r="A20" s="2"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="54">
+        <v>17</v>
+      </c>
+      <c r="C20" s="54">
+        <v>9</v>
+      </c>
+      <c r="D20" s="54">
+        <v>5</v>
+      </c>
+      <c r="E20" s="54">
+        <v>4</v>
+      </c>
+      <c r="F20" s="54">
+        <v>2</v>
+      </c>
+      <c r="G20" s="26"/>
       <c r="H20" s="14"/>
       <c r="I20" s="5">
         <f t="shared" si="0"/>
@@ -1798,48 +1895,61 @@
       </c>
       <c r="J20" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="K20" s="5">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <f t="shared" ref="K12:K29" si="8">MIN(1+(ROUNDDOWN(((I20-J20))/(I20/20),0)*(1/3)),5)</f>
+        <v>2.6666666666666665</v>
       </c>
       <c r="L20" s="5">
-        <f t="shared" si="9"/>
-        <v>20</v>
+        <f t="shared" ref="L12:L29" si="9">IF(K20&gt;1, I20 - ((K20-1) * 3 * (I20 / 20)) - J20, "X")</f>
+        <v>0.5</v>
       </c>
       <c r="M20" s="14"/>
-      <c r="N20" s="1">
+      <c r="N20" s="72">
         <v>10</v>
       </c>
       <c r="O20" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="Q12:Q29" si="10">I20+N$2+O$2</f>
         <v>100</v>
       </c>
       <c r="R20" s="5">
         <f>IF(ISNUMBER(#REF!), J20*0.8+#REF! +N20+O20, J20+N20+O20)</f>
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="S20" s="5">
-        <f t="shared" si="11"/>
-        <v>4.333333333333333</v>
+        <f t="shared" ref="S12:S29" si="11">MIN(1+(ROUNDDOWN(((Q20-R20))/(Q20/20),0)*(1/3)),5)</f>
+        <v>2.333333333333333</v>
       </c>
       <c r="T20" s="5">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" ref="T12:T29" si="12">IF(S20&gt;1, Q20 - ((S20-1) * 3 * (Q20 / 20)) - R20, "X")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="15">
-      <c r="A21" s="2"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
+      <c r="A21" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="54">
+        <v>14</v>
+      </c>
+      <c r="C21" s="54">
+        <v>6</v>
+      </c>
+      <c r="D21" s="54">
+        <v>5</v>
+      </c>
+      <c r="E21" s="54">
+        <v>2</v>
+      </c>
+      <c r="F21" s="54">
+        <v>2</v>
+      </c>
+      <c r="G21" s="26"/>
       <c r="H21" s="14"/>
       <c r="I21" s="5">
         <f t="shared" si="0"/>
@@ -1847,19 +1957,22 @@
       </c>
       <c r="J21" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="M21" s="14"/>
-      <c r="N21" s="1">
-        <v>0</v>
+      <c r="N21" s="71">
+        <v>10</v>
+      </c>
+      <c r="O21" s="1">
+        <v>33</v>
       </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="5">
@@ -1868,124 +1981,133 @@
       </c>
       <c r="R21" s="5">
         <f>IF(ISNUMBER(#REF!), J21*0.8+#REF! +N21+O21, J21+N21+O21)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="S21" s="5">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="T21" s="5">
         <f t="shared" si="12"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="15">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="74">
+        <v>24</v>
+      </c>
+      <c r="C22" s="74">
+        <v>9</v>
+      </c>
+      <c r="D22" s="74">
+        <v>5</v>
+      </c>
+      <c r="E22" s="74">
+        <v>4</v>
+      </c>
+      <c r="F22" s="74">
+        <v>3</v>
+      </c>
+      <c r="G22" s="42"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="44">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="K22" s="44">
+        <f t="shared" si="8"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="L22" s="44">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="43"/>
+      <c r="N22" s="75">
+        <v>10</v>
+      </c>
+      <c r="O22" s="45">
+        <v>37</v>
+      </c>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="44">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="R22" s="44">
+        <f>IF(ISNUMBER(#REF!), J22*0.8+#REF! +N22+O22, J22+N22+O22)</f>
+        <v>92</v>
+      </c>
+      <c r="S22" s="44">
+        <f t="shared" si="11"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="T22" s="44">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="37"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="37">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J23" s="37">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K23" s="40">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="L22" s="20">
+      <c r="L23" s="37">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
-      <c r="M22" s="19"/>
-      <c r="N22" s="18">
-        <v>8</v>
-      </c>
-      <c r="O22" s="18">
-        <v>20</v>
-      </c>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="20">
+      <c r="M23" s="39"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="37">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R22" s="20">
-        <f>IF(ISNUMBER(#REF!), J22*0.8+#REF! +N22+O22, J22+N22+O22)</f>
-        <v>28</v>
-      </c>
-      <c r="S22" s="20">
+      <c r="R23" s="37">
+        <f>IF(ISNUMBER(#REF!), J23*0.8+#REF! +N23+O23, J23+N23+O23)</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="40">
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="T22" s="20">
+      <c r="T23" s="37">
         <f t="shared" si="12"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="21">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J23" s="21">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="23">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="L23" s="21">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="M23" s="22"/>
-      <c r="N23" s="21">
-        <v>5</v>
-      </c>
-      <c r="O23" s="21">
-        <v>21</v>
-      </c>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="21">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="R23" s="21">
-        <f>IF(ISNUMBER(#REF!), J23*0.8+#REF! +N23+O23, J23+N23+O23)</f>
-        <v>26</v>
-      </c>
-      <c r="S23" s="23">
-        <f t="shared" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="T23" s="21">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15">
       <c r="A24" s="2"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="14"/>
       <c r="I24" s="5">
         <f t="shared" si="0"/>
@@ -2004,12 +2126,7 @@
         <v>20</v>
       </c>
       <c r="M24" s="14"/>
-      <c r="N24" s="1">
-        <v>10</v>
-      </c>
-      <c r="O24" s="1">
-        <v>40</v>
-      </c>
+      <c r="N24" s="31"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="5">
         <f t="shared" si="10"/>
@@ -2017,24 +2134,25 @@
       </c>
       <c r="R24" s="5">
         <f>IF(ISNUMBER(#REF!), J24*0.8+#REF! +N24+O24, J24+N24+O24)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S24" s="5">
         <f t="shared" si="11"/>
-        <v>4.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="T24" s="5">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="15">
       <c r="A25" s="2"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="14"/>
       <c r="I25" s="5">
         <f t="shared" si="0"/>
@@ -2053,12 +2171,7 @@
         <v>20</v>
       </c>
       <c r="M25" s="14"/>
-      <c r="N25" s="1">
-        <v>10</v>
-      </c>
-      <c r="O25" s="1">
-        <v>40</v>
-      </c>
+      <c r="N25" s="31"/>
       <c r="P25" s="14"/>
       <c r="Q25" s="5">
         <f t="shared" si="10"/>
@@ -2066,24 +2179,25 @@
       </c>
       <c r="R25" s="5">
         <f>IF(ISNUMBER(#REF!), J25*0.8+#REF! +N25+O25, J25+N25+O25)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S25" s="5">
         <f t="shared" si="11"/>
-        <v>4.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="T25" s="5">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="15">
       <c r="A26" s="2"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
       <c r="H26" s="14"/>
       <c r="I26" s="5">
         <f t="shared" si="0"/>
@@ -2102,12 +2216,7 @@
         <v>20</v>
       </c>
       <c r="M26" s="14"/>
-      <c r="N26" s="1">
-        <v>10</v>
-      </c>
-      <c r="O26" s="1">
-        <v>40</v>
-      </c>
+      <c r="N26" s="31"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="5">
         <f t="shared" si="10"/>
@@ -2115,74 +2224,71 @@
       </c>
       <c r="R26" s="5">
         <f>IF(ISNUMBER(#REF!), J26*0.8+#REF! +N26+O26, J26+N26+O26)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S26" s="5">
         <f t="shared" si="11"/>
-        <v>4.333333333333333</v>
+        <v>5</v>
       </c>
       <c r="T26" s="5">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="15">
       <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="19">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="J27" s="20">
+      <c r="J27" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K27" s="20">
+      <c r="K27" s="19">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="L27" s="20">
+      <c r="L27" s="19">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
-      <c r="M27" s="19"/>
-      <c r="N27" s="18">
-        <v>7</v>
-      </c>
-      <c r="O27" s="18">
-        <v>36</v>
-      </c>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="20">
+      <c r="M27" s="18"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="19">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R27" s="20">
+      <c r="R27" s="19">
         <f>IF(ISNUMBER(#REF!), J27*0.8+#REF! +N27+O27, J27+N27+O27)</f>
-        <v>43</v>
-      </c>
-      <c r="S27" s="20">
+        <v>0</v>
+      </c>
+      <c r="S27" s="19">
         <f t="shared" si="11"/>
-        <v>4.6666666666666661</v>
-      </c>
-      <c r="T27" s="20">
+        <v>5</v>
+      </c>
+      <c r="T27" s="19">
         <f t="shared" si="12"/>
-        <v>2.0000000000000071</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15">
       <c r="A28" s="2"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="14"/>
       <c r="I28" s="5">
         <f t="shared" si="0"/>
@@ -2201,12 +2307,7 @@
         <v>20</v>
       </c>
       <c r="M28" s="14"/>
-      <c r="N28" s="1">
-        <v>7</v>
-      </c>
-      <c r="O28" s="1">
-        <v>28</v>
-      </c>
+      <c r="N28" s="31"/>
       <c r="P28" s="14"/>
       <c r="Q28" s="5">
         <f t="shared" si="10"/>
@@ -2214,7 +2315,7 @@
       </c>
       <c r="R28" s="5">
         <f>IF(ISNUMBER(#REF!), J28*0.8+#REF! +N28+O28, J28+N28+O28)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="S28" s="5">
         <f t="shared" si="11"/>
@@ -2222,73 +2323,67 @@
       </c>
       <c r="T28" s="5">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="21">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J29" s="21">
-        <f t="shared" si="7"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="20">
+        <v>40</v>
+      </c>
+      <c r="J29" s="20">
+        <v>36</v>
+      </c>
+      <c r="K29" s="22">
+        <f t="shared" si="8"/>
+        <v>1.6666666666666665</v>
+      </c>
+      <c r="L29" s="20">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K29" s="23">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="L29" s="21">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="M29" s="22"/>
-      <c r="N29" s="21">
-        <v>7</v>
-      </c>
-      <c r="O29" s="21">
-        <v>32</v>
-      </c>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="21">
+      <c r="M29" s="21"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="20">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="R29" s="21">
+        <v>90</v>
+      </c>
+      <c r="R29" s="20">
         <f>IF(ISNUMBER(#REF!), J29*0.8+#REF! +N29+O29, J29+N29+O29)</f>
-        <v>39</v>
-      </c>
-      <c r="S29" s="23">
+        <v>36</v>
+      </c>
+      <c r="S29" s="22">
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="T29" s="21">
+      <c r="T29" s="20">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:20">
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
       <c r="L30"/>
       <c r="M30"/>
-      <c r="N30"/>
+      <c r="N30" s="31"/>
       <c r="O30"/>
       <c r="P30"/>
       <c r="Q30"/>
@@ -2402,7 +2497,10 @@
       <c r="T35" s="5"/>
     </row>
     <row r="36" spans="2:20">
-      <c r="B36"/>
+      <c r="B36" s="31">
+        <f>SUM(B5:F5)</f>
+        <v>50</v>
+      </c>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>

</xml_diff>